<commit_message>
update bau gra settings for carbon tax
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\Canada\eps-canada\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA381170-8E27-40B4-9CBD-1B52CDE9D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2670" windowWidth="25665" windowHeight="13515" tabRatio="698"/>
+    <workbookView xWindow="315" yWindow="200" windowWidth="10390" windowHeight="9805" tabRatio="698" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <sheet name="GRA-ntnldebtinterest" sheetId="15" r:id="rId10"/>
     <sheet name="GRA-remainder" sheetId="16" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,6 +36,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,26 +46,17 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={4F81BCB5-E56D-426A-91DB-BCF0877CB817}</author>
   </authors>
   <commentList>
-    <comment ref="C15" authorId="0" shapeId="0">
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     It is recommended to leave this cell set to zero and to set a non-zero value in at least one other cell in this row.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -272,7 +267,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,7 +375,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -713,22 +708,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="80.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,72 +731,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -809,7 +804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -817,7 +812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -825,7 +820,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -833,7 +828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -841,114 +836,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -960,7 +955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -968,12 +963,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -981,7 +976,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -990,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -998,7 +993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1006,7 +1001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1014,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1028,7 +1023,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1036,12 +1031,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1044,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1058,7 +1053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1066,7 +1061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1074,7 +1069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1082,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1096,7 +1091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1106,33 +1101,33 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1142,7 +1137,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1162,7 +1157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1182,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1202,7 +1197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1222,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1242,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1262,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1282,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1322,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1342,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1352,12 +1347,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1377,7 +1372,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1402,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1427,7 +1422,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1452,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1477,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1502,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1527,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1552,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1577,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1610,22 +1605,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1633,16 +1628,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1650,23 +1644,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1680,7 +1674,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1690,12 +1684,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1703,7 +1697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1712,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1720,7 +1714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1728,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1736,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1750,7 +1744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1758,12 +1752,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1771,7 +1765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1780,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1788,7 +1782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1796,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1804,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1818,7 +1812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1826,12 +1820,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1839,7 +1833,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1848,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1856,7 +1850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1864,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1872,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1886,7 +1880,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1894,12 +1888,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1907,7 +1901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1916,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1924,7 +1918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1932,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1940,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1954,7 +1948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1962,12 +1956,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1975,7 +1969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1984,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1992,7 +1986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2000,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2008,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2022,7 +2016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2030,12 +2024,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2043,7 +2037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2052,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2060,7 +2054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2068,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2076,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Revert "update bau gra settings for carbon tax"
This reverts commit e87721408690767b52f8d7c38730c599ac7d0a4a.
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\Canada\eps-canada\InputData\ctrl-settings\GRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA381170-8E27-40B4-9CBD-1B52CDE9D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="200" windowWidth="10390" windowHeight="9805" tabRatio="698" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="2670" windowWidth="25665" windowHeight="13515" tabRatio="698"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="GRA-ntnldebtinterest" sheetId="15" r:id="rId10"/>
     <sheet name="GRA-remainder" sheetId="16" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +35,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,17 +42,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={4F81BCB5-E56D-426A-91DB-BCF0877CB817}</author>
   </authors>
   <commentList>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="C15" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     It is recommended to leave this cell set to zero and to set a non-zero value in at least one other cell in this row.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -267,7 +272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,7 +380,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -708,22 +713,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="80.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -731,72 +736,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -804,7 +809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -812,7 +817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -820,7 +825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -828,7 +833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -836,114 +841,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -955,7 +960,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -963,12 +968,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -976,7 +981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -985,7 +990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -993,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1001,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1009,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1023,7 +1028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1031,12 +1036,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1044,7 +1049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1053,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1069,7 +1074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1077,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1091,7 +1096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1101,33 +1106,33 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1137,7 +1142,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1157,7 +1162,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1177,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1197,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1217,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1237,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1257,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1277,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1297,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1317,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1337,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1347,12 +1352,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1372,7 +1377,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1397,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1422,7 +1427,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1447,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1472,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1497,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1522,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1547,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1572,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1605,22 +1610,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1628,15 +1633,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+        <f t="array" ref="B2:B6">TRANSPOSE('Set Values Here'!B8:F8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1644,23 +1650,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1674,7 +1680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1684,12 +1690,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1697,7 +1703,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1706,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1722,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1744,7 +1750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1752,12 +1758,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1812,7 +1818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1820,12 +1826,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1833,7 +1839,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1850,7 +1856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1858,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1866,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1880,7 +1886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1888,12 +1894,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1901,7 +1907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1918,7 +1924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1926,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1934,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1948,7 +1954,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1956,12 +1962,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1969,7 +1975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1978,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1986,7 +1992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2016,7 +2022,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2024,12 +2030,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2037,7 +2043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2046,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2054,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>

</xml_diff>